<commit_message>
Update of ch2//chip-seq draft
</commit_message>
<xml_diff>
--- a/data/timepoint_information.xlsx
+++ b/data/timepoint_information.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28080" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="780" windowWidth="28080" windowHeight="16820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="dafka2" localSheetId="0">Sheet1!$B$8</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>BOWNES STAGES:</t>
   </si>
@@ -234,6 +235,15 @@
   </si>
   <si>
     <t>Stages</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>t3</t>
   </si>
 </sst>
 </file>
@@ -586,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -922,4 +932,91 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1">
+        <v>782</v>
+      </c>
+      <c r="G1">
+        <f>E1/SUM(E1:E3)</f>
+        <v>0.50031989763275753</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4">
+        <v>3056</v>
+      </c>
+      <c r="G4">
+        <f>E4/SUM(E2:E5)</f>
+        <v>0.58253907739229893</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6">
+        <v>2311</v>
+      </c>
+      <c r="G6">
+        <f>E6/SUM(E6,E5,E3)</f>
+        <v>0.52084741942754109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>